<commit_message>
Update Comparisons Of Machine Learning, Deep Learning And Reinforcement Learning Libraries.xlsx
</commit_message>
<xml_diff>
--- a/Comparisons Of Machine Learning, Deep Learning And Reinforcement Learning Libraries.xlsx
+++ b/Comparisons Of Machine Learning, Deep Learning And Reinforcement Learning Libraries.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aqwam\Documents\GitHub\Software-Libraries-Comparisons\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C2E20EE-A74D-43FB-A918-C9FF6E12C72F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED40EC51-F682-4E19-B49D-A296A87014C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="77">
   <si>
     <t>MyOriginsWorkshop (Aqwam Harish Aiman)</t>
   </si>
@@ -210,9 +210,6 @@
   </si>
   <si>
     <t>Average Training Speed For Neural Networks (in seconds)</t>
-  </si>
-  <si>
-    <t>Partial</t>
   </si>
   <si>
     <t>Reinforcement Learning Support</t>
@@ -604,7 +601,7 @@
   <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="50.7109375" defaultRowHeight="60" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -614,7 +611,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -637,7 +634,7 @@
     </row>
     <row r="2" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>0</v>
@@ -660,7 +657,7 @@
     </row>
     <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>54</v>
@@ -683,7 +680,7 @@
     </row>
     <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>55</v>
@@ -732,13 +729,13 @@
         <v>17</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>58</v>
+        <v>19</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>18</v>
@@ -752,10 +749,10 @@
     </row>
     <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>13</v>
@@ -764,7 +761,7 @@
         <v>15</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>15</v>
@@ -775,10 +772,10 @@
     </row>
     <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>13</v>
@@ -916,13 +913,13 @@
         <v>33</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>15</v>
@@ -965,13 +962,13 @@
         <v>39</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>39</v>
@@ -1028,7 +1025,7 @@
     </row>
     <row r="19" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B19" s="1">
         <f xml:space="preserve"> $B$18 / B18</f>
@@ -1095,15 +1092,15 @@
         <v>45</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>2</v>
@@ -1152,7 +1149,7 @@
         <v>49</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>13</v>

</xml_diff>